<commit_message>
modified simple excel output
</commit_message>
<xml_diff>
--- a/BL_simple.xlsx
+++ b/BL_simple.xlsx
@@ -477,10 +477,10 @@
         <v>0.5</v>
       </c>
       <c r="C3">
-        <v>1.4117828395613839E-2</v>
+        <v>1.4117828395613858E-2</v>
       </c>
       <c r="D3">
-        <v>1.0097423249785198</v>
+        <v>1.0097423249785216</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -491,10 +491,10 @@
         <v>0.4</v>
       </c>
       <c r="C4">
-        <v>1.8731041839192497E-2</v>
+        <v>1.8731041839192504E-2</v>
       </c>
       <c r="D4">
-        <v>1.382837853833303</v>
+        <v>1.3828378538332984</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -505,10 +505,10 @@
         <v>0.1</v>
       </c>
       <c r="C5">
-        <v>-8.433344253473014E-3</v>
+        <v>-8.4333442534729984E-3</v>
       </c>
       <c r="D5">
-        <v>-1.3925801788118226</v>
+        <v>-1.3925801788118197</v>
       </c>
     </row>
   </sheetData>
@@ -638,32 +638,32 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1.8624405565223962E-3</v>
+        <v>1.8624405565223958E-3</v>
       </c>
       <c r="B2">
-        <v>1.6131321148877217E-3</v>
+        <v>1.6131321148877219E-3</v>
       </c>
       <c r="C2">
-        <v>2.0494648500952914E-3</v>
+        <v>2.0494648500952919E-3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1.6131321148877217E-3</v>
+        <v>1.6131321148877219E-3</v>
       </c>
       <c r="B3">
         <v>2.460197306144522E-3</v>
       </c>
       <c r="C3">
-        <v>2.4148255238334057E-3</v>
+        <v>2.4148255238334053E-3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2.0494648500952914E-3</v>
+        <v>2.0494648500952919E-3</v>
       </c>
       <c r="B4">
-        <v>2.4148255238334057E-3</v>
+        <v>2.4148255238334053E-3</v>
       </c>
       <c r="C4">
         <v>4.423272639325522E-3</v>
@@ -697,10 +697,10 @@
         <v>16</v>
       </c>
       <c r="B2">
-        <v>5.7879615895029589E-3</v>
+        <v>5.7879615895029598E-3</v>
       </c>
       <c r="C2">
-        <v>5.1901470613288744E-2</v>
+        <v>5.1901470613288668E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -708,10 +708,10 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>1.9293205298343196E-3</v>
+        <v>1.9293205298343199E-3</v>
       </c>
       <c r="C3">
-        <v>4.6220041242065685E-3</v>
+        <v>4.622004124206552E-3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -722,7 +722,7 @@
         <v>4.3924031347706685E-2</v>
       </c>
       <c r="C4">
-        <v>6.7985322858735972E-2</v>
+        <v>6.7985322858735861E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -733,7 +733,7 @@
         <v>0.13177209404312007</v>
       </c>
       <c r="C5">
-        <v>0.76342169796167281</v>
+        <v>0.76342169796167292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>